<commit_message>
fix: data POST formSPT-TS, export to excel, schema TS
</commit_message>
<xml_diff>
--- a/tracerStudy.xlsx
+++ b/tracerStudy.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Trace Study" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Data Tracer Study" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="203">
   <si>
     <t>kdptimsmh</t>
   </si>
@@ -539,6 +539,87 @@
   </si>
   <si>
     <t>data.f1614</t>
+  </si>
+  <si>
+    <t>161002</t>
+  </si>
+  <si>
+    <t>57201</t>
+  </si>
+  <si>
+    <t>20502201008</t>
+  </si>
+  <si>
+    <t>Sheilakathryn Heppner</t>
+  </si>
+  <si>
+    <t>081234567899</t>
+  </si>
+  <si>
+    <t>sheila@contoh.com</t>
+  </si>
+  <si>
+    <t>2022</t>
+  </si>
+  <si>
+    <t>7171098765432100</t>
+  </si>
+  <si>
+    <t>01.234.567.8-123.000</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2 Bulan</t>
+  </si>
+  <si>
+    <t>Rp 1.000.000</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Sulawesi Utara</t>
+  </si>
+  <si>
+    <t>Kota Manado</t>
+  </si>
+  <si>
+    <t>Klabat Tekno</t>
+  </si>
+  <si>
+    <t>CEO</t>
+  </si>
+  <si>
+    <t>Tinggi</t>
+  </si>
+  <si>
+    <t>Orang Tua</t>
+  </si>
+  <si>
+    <t>Universitas Klabat</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>12/01/2026</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -915,7 +996,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ16"/>
+  <dimension ref="A1:CJ17"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:88" x14ac:dyDescent="0.25">
@@ -5172,6 +5253,272 @@
       </c>
       <c r="CJ16" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>176</v>
+      </c>
+      <c r="B17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C17" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" t="s">
+        <v>179</v>
+      </c>
+      <c r="E17" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" t="s">
+        <v>181</v>
+      </c>
+      <c r="G17" t="s">
+        <v>182</v>
+      </c>
+      <c r="H17" t="s">
+        <v>183</v>
+      </c>
+      <c r="I17" t="s">
+        <v>184</v>
+      </c>
+      <c r="J17" t="s">
+        <v>185</v>
+      </c>
+      <c r="K17" t="s">
+        <v>185</v>
+      </c>
+      <c r="L17" t="s">
+        <v>186</v>
+      </c>
+      <c r="M17" t="s">
+        <v>187</v>
+      </c>
+      <c r="N17" t="s">
+        <v>188</v>
+      </c>
+      <c r="O17" t="s">
+        <v>189</v>
+      </c>
+      <c r="P17" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>185</v>
+      </c>
+      <c r="R17" t="s">
+        <v>188</v>
+      </c>
+      <c r="S17" t="s">
+        <v>191</v>
+      </c>
+      <c r="T17" t="s">
+        <v>192</v>
+      </c>
+      <c r="U17" t="s">
+        <v>193</v>
+      </c>
+      <c r="V17" t="s">
+        <v>194</v>
+      </c>
+      <c r="W17" t="s">
+        <v>195</v>
+      </c>
+      <c r="X17" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>188</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>199</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>200</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>201</v>
+      </c>
+      <c r="AI17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AJ17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AK17" t="s">
+        <v>199</v>
+      </c>
+      <c r="AL17" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM17" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AO17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AP17" t="s">
+        <v>199</v>
+      </c>
+      <c r="AQ17" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AS17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AT17" t="s">
+        <v>199</v>
+      </c>
+      <c r="AU17" t="s">
+        <v>200</v>
+      </c>
+      <c r="AV17" t="s">
+        <v>201</v>
+      </c>
+      <c r="AW17" t="s">
+        <v>198</v>
+      </c>
+      <c r="AX17" t="s">
+        <v>200</v>
+      </c>
+      <c r="AY17" t="s">
+        <v>199</v>
+      </c>
+      <c r="AZ17" t="s">
+        <v>188</v>
+      </c>
+      <c r="BA17" t="s">
+        <v>188</v>
+      </c>
+      <c r="BB17" t="s">
+        <v>185</v>
+      </c>
+      <c r="BC17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BD17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BE17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BF17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BG17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BH17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BI17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BJ17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BK17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BL17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BM17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BN17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BO17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BP17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BQ17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BR17" t="s">
+        <v>198</v>
+      </c>
+      <c r="BS17" t="s">
+        <v>185</v>
+      </c>
+      <c r="BT17" t="s">
+        <v>185</v>
+      </c>
+      <c r="BU17" t="s">
+        <v>200</v>
+      </c>
+      <c r="BV17" t="s">
+        <v>188</v>
+      </c>
+      <c r="BW17" t="s">
+        <v>185</v>
+      </c>
+      <c r="BX17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BY17" t="s">
+        <v>202</v>
+      </c>
+      <c r="BZ17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CA17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CB17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CC17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CD17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CE17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CF17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CG17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CH17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CI17" t="s">
+        <v>202</v>
+      </c>
+      <c r="CJ17" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: broadcast email and whatsapp
</commit_message>
<xml_diff>
--- a/tracerStudy.xlsx
+++ b/tracerStudy.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1496" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1408" uniqueCount="176">
   <si>
     <t>kdptimsmh</t>
   </si>
@@ -539,87 +539,6 @@
   </si>
   <si>
     <t>data.f1614</t>
-  </si>
-  <si>
-    <t>161002</t>
-  </si>
-  <si>
-    <t>57201</t>
-  </si>
-  <si>
-    <t>20502201008</t>
-  </si>
-  <si>
-    <t>Sheilakathryn Heppner</t>
-  </si>
-  <si>
-    <t>081234567899</t>
-  </si>
-  <si>
-    <t>sheila@contoh.com</t>
-  </si>
-  <si>
-    <t>2022</t>
-  </si>
-  <si>
-    <t>7171098765432100</t>
-  </si>
-  <si>
-    <t>01.234.567.8-123.000</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2 Bulan</t>
-  </si>
-  <si>
-    <t>Rp 1.000.000</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Sulawesi Utara</t>
-  </si>
-  <si>
-    <t>Kota Manado</t>
-  </si>
-  <si>
-    <t>Klabat Tekno</t>
-  </si>
-  <si>
-    <t>CEO</t>
-  </si>
-  <si>
-    <t>Tinggi</t>
-  </si>
-  <si>
-    <t>Orang Tua</t>
-  </si>
-  <si>
-    <t>Universitas Klabat</t>
-  </si>
-  <si>
-    <t>Management</t>
-  </si>
-  <si>
-    <t>12/01/2026</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>0</t>
   </si>
 </sst>
 </file>
@@ -996,7 +915,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CJ17"/>
+  <dimension ref="A1:CJ16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:88" x14ac:dyDescent="0.25">
@@ -5253,272 +5172,6 @@
       </c>
       <c r="CJ16" t="s">
         <v>175</v>
-      </c>
-    </row>
-    <row r="17" spans="1:88" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>176</v>
-      </c>
-      <c r="B17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E17" t="s">
-        <v>180</v>
-      </c>
-      <c r="F17" t="s">
-        <v>181</v>
-      </c>
-      <c r="G17" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" t="s">
-        <v>183</v>
-      </c>
-      <c r="I17" t="s">
-        <v>184</v>
-      </c>
-      <c r="J17" t="s">
-        <v>185</v>
-      </c>
-      <c r="K17" t="s">
-        <v>185</v>
-      </c>
-      <c r="L17" t="s">
-        <v>186</v>
-      </c>
-      <c r="M17" t="s">
-        <v>187</v>
-      </c>
-      <c r="N17" t="s">
-        <v>188</v>
-      </c>
-      <c r="O17" t="s">
-        <v>189</v>
-      </c>
-      <c r="P17" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>185</v>
-      </c>
-      <c r="R17" t="s">
-        <v>188</v>
-      </c>
-      <c r="S17" t="s">
-        <v>191</v>
-      </c>
-      <c r="T17" t="s">
-        <v>192</v>
-      </c>
-      <c r="U17" t="s">
-        <v>193</v>
-      </c>
-      <c r="V17" t="s">
-        <v>194</v>
-      </c>
-      <c r="W17" t="s">
-        <v>195</v>
-      </c>
-      <c r="X17" t="s">
-        <v>196</v>
-      </c>
-      <c r="Y17" t="s">
-        <v>197</v>
-      </c>
-      <c r="Z17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AA17" t="s">
-        <v>188</v>
-      </c>
-      <c r="AB17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AC17" t="s">
-        <v>198</v>
-      </c>
-      <c r="AD17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AE17" t="s">
-        <v>198</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>199</v>
-      </c>
-      <c r="AG17" t="s">
-        <v>200</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>201</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>198</v>
-      </c>
-      <c r="AK17" t="s">
-        <v>199</v>
-      </c>
-      <c r="AL17" t="s">
-        <v>200</v>
-      </c>
-      <c r="AM17" t="s">
-        <v>201</v>
-      </c>
-      <c r="AN17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AO17" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP17" t="s">
-        <v>199</v>
-      </c>
-      <c r="AQ17" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AS17" t="s">
-        <v>198</v>
-      </c>
-      <c r="AT17" t="s">
-        <v>199</v>
-      </c>
-      <c r="AU17" t="s">
-        <v>200</v>
-      </c>
-      <c r="AV17" t="s">
-        <v>201</v>
-      </c>
-      <c r="AW17" t="s">
-        <v>198</v>
-      </c>
-      <c r="AX17" t="s">
-        <v>200</v>
-      </c>
-      <c r="AY17" t="s">
-        <v>199</v>
-      </c>
-      <c r="AZ17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BA17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BB17" t="s">
-        <v>185</v>
-      </c>
-      <c r="BC17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BD17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BE17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BF17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BG17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BH17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BI17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BJ17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BK17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BL17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BM17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BN17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BO17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BP17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BQ17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BR17" t="s">
-        <v>198</v>
-      </c>
-      <c r="BS17" t="s">
-        <v>185</v>
-      </c>
-      <c r="BT17" t="s">
-        <v>185</v>
-      </c>
-      <c r="BU17" t="s">
-        <v>200</v>
-      </c>
-      <c r="BV17" t="s">
-        <v>188</v>
-      </c>
-      <c r="BW17" t="s">
-        <v>185</v>
-      </c>
-      <c r="BX17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BY17" t="s">
-        <v>202</v>
-      </c>
-      <c r="BZ17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CA17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CB17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CC17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CD17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CE17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CF17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CG17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CH17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CI17" t="s">
-        <v>202</v>
-      </c>
-      <c r="CJ17" t="s">
-        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>